<commit_message>
working on hybrid method, hodgepodge of updates
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="6384"/>
+    <workbookView xWindow="380" yWindow="80" windowWidth="16260" windowHeight="6380"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t xml:space="preserve">Expand possible areas for trouble-shooting help: non posdef, no sd.report variables, bounds issues </t>
+  </si>
+  <si>
+    <t>What is option -mcec? What is empirical covariance?</t>
+  </si>
+  <si>
+    <t>What is the .bgs file used for? Read in if mcmc2_flag==TRUE</t>
+  </si>
+  <si>
+    <t>Deduce which options are available for the hybrid method</t>
   </si>
 </sst>
 </file>
@@ -496,22 +505,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G21"/>
+  <dimension ref="B3:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="53.88671875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="13.109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="74.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="53.90625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="13.08984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="74.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,12 +537,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -547,7 +556,7 @@
         <v>41829</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -555,7 +564,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -566,7 +575,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -577,7 +586,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
@@ -588,7 +597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -599,7 +608,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
@@ -607,7 +616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
@@ -615,7 +624,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
@@ -626,7 +635,7 @@
         <v>41838</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -637,7 +646,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -645,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -656,7 +665,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
@@ -664,7 +673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -675,7 +684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -686,14 +695,29 @@
         <v>41838</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="28.75" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -709,10 +733,10 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="66.44140625" customWidth="1"/>
-    <col min="4" max="4" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.453125" customWidth="1"/>
+    <col min="4" max="4" width="68.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated checklist, added a few new items
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Task</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>See next sheet</t>
+  </si>
+  <si>
+    <t>Add section about seeds/reproducibility</t>
+  </si>
+  <si>
+    <t>Mention capabilities of R2admb</t>
+  </si>
+  <si>
+    <t>define what mcmult argument does</t>
   </si>
 </sst>
 </file>
@@ -549,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G24"/>
+  <dimension ref="B3:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,8 +641,8 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8">
-        <v>0.5</v>
+      <c r="D8" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -798,7 +807,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="14.55" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:6" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added proposed changes to checklist
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="6384" activeTab="1"/>
+    <workbookView xWindow="380" yWindow="80" windowWidth="16260" windowHeight="6380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t>Task</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Not really sure; perhaps suggest this be renamed to bounded_flag since it has nothing to do with the hybrid method.</t>
+  </si>
+  <si>
+    <t>http://admb-project.org/documentation/api/xxmcmc_8cpp_source.html#l00627</t>
+  </si>
+  <si>
+    <t>More informative output for MCMC, especially the -objective fn value (llc)</t>
   </si>
 </sst>
 </file>
@@ -585,16 +591,16 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="53.88671875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="13.109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="74.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="53.90625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="13.08984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="74.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -622,7 +628,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -636,7 +642,7 @@
         <v>41829</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -647,7 +653,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -661,7 +667,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -672,7 +678,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
@@ -683,7 +689,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -694,7 +700,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
@@ -708,7 +714,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
@@ -716,7 +722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
@@ -733,7 +739,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -744,7 +750,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -755,7 +761,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -769,7 +775,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
@@ -780,7 +786,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -794,7 +800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -805,7 +811,7 @@
         <v>41838</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
@@ -819,7 +825,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="28.75" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>35</v>
       </c>
@@ -827,7 +833,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
@@ -841,17 +847,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>57</v>
       </c>
@@ -866,13 +872,13 @@
   <dimension ref="C2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="66.44140625" customWidth="1"/>
-    <col min="4" max="4" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.453125" customWidth="1"/>
+    <col min="4" max="4" width="68.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.3">
@@ -930,6 +936,14 @@
         <v>59</v>
       </c>
     </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>39</v>
@@ -954,6 +968,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" location="l00147"/>
+    <hyperlink ref="D12" r:id="rId2" location="l00627"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
started final edit, need to finish still
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13980" activeTab="1"/>
+    <workbookView xWindow="564" yWindow="564" windowWidth="25044" windowHeight="13980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t>Task</t>
   </si>
@@ -206,6 +206,21 @@
   </si>
   <si>
     <t>I totally agree with these, maybe add a section to the hst file called MCMC stats. I also think adding the ability to write the unscaled hist values, or maybe even each saved value, to a binary file (similar to the psv file) would be really helpful so that users can read in their saved param values from one file and their saved sdreport values from another. Of course the user can do it with an IO object, but I bet writing it to a binary file is hella faster - Melissa</t>
+  </si>
+  <si>
+    <t>Therefore, we propose a few
+improvements to the general usability of the \texttt{.hst} file: adding elements that
+report the date and time that the associated MCMC chain was started, the
+\texttt{-mcsave $nsave$} used, and the date and time the chain finished would be useful
+data to have associated with each chain.</t>
+  </si>
+  <si>
+    <t>We would like to recommend a user-friendly addition to the ADMB output files:
+something like an \texttt{.sdsv} file that would be similar to the \texttt{.psv}
+file, in that each saved \texttt{sdreport} value is written to a binary file. This
+file could then be read into R using the same code as for the \texttt{.psv} file
+and used to create histograms of the posterior distributions and calculate the
+median and credible intervals for each \texttt{sdreport} vaariable.</t>
   </si>
 </sst>
 </file>
@@ -593,16 +608,16 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.83203125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="13.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="74.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="4"/>
+    <col min="2" max="2" width="53.77734375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="13.109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="74.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -630,7 +645,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -644,7 +659,7 @@
         <v>41829</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -655,7 +670,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -669,7 +684,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -680,7 +695,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
@@ -691,7 +706,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -702,7 +717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
@@ -716,7 +731,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>50</v>
       </c>
@@ -724,7 +739,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
@@ -741,7 +756,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -752,7 +767,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
@@ -763,7 +778,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -777,7 +792,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
@@ -788,7 +803,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -802,7 +817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -816,7 +831,7 @@
         <v>41838</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
@@ -830,7 +845,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="28">
+    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>34</v>
       </c>
@@ -838,7 +853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
@@ -852,7 +867,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>47</v>
       </c>
@@ -872,30 +887,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D16"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="57.83203125" customWidth="1"/>
-    <col min="3" max="3" width="68.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57.77734375" customWidth="1"/>
+    <col min="3" max="3" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.6640625" customWidth="1"/>
+    <col min="5" max="5" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -903,7 +919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -911,7 +927,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="84">
+    <row r="8" spans="2:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -921,21 +937,27 @@
       <c r="D8" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="2:4">
+      <c r="E8" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="E9" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>53</v>
       </c>
@@ -943,7 +965,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>58</v>
       </c>
@@ -951,12 +973,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -964,7 +986,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>40</v>
       </c>

</xml_diff>